<commit_message>
commit cái đéo gì đó
</commit_message>
<xml_diff>
--- a/Sprite Soures/temp_push.xlsx
+++ b/Sprite Soures/temp_push.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:I2"/>
+      <selection activeCell="I6" sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,7 +366,7 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B10" si="0">M1</f>
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -380,14 +380,14 @@
       </c>
       <c r="F1">
         <f t="shared" ref="F1:F10" si="2">M1+O1</f>
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1">
         <f t="shared" ref="H1:H10" si="3">L1+N1</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -402,13 +402,13 @@
         <v>0</v>
       </c>
       <c r="M1">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="N1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O1">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -424,21 +424,21 @@
       </c>
       <c r="D2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
@@ -450,16 +450,16 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O2">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -468,28 +468,28 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
@@ -501,16 +501,16 @@
         <v>0</v>
       </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>33</v>
+      </c>
+      <c r="N3">
         <v>31</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>30</v>
-      </c>
       <c r="O3">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -526,21 +526,21 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
@@ -552,16 +552,16 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -570,28 +570,28 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
@@ -603,16 +603,16 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N5">
         <v>30</v>
       </c>
       <c r="O5">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -635,14 +635,14 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
@@ -657,10 +657,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="O6">
         <v>32</v>
@@ -672,28 +672,28 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
         <v>2</v>
@@ -705,16 +705,16 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="N7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O7">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -744,13 +744,13 @@
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>34</v>
       </c>
       <c r="N8">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O8">
         <v>34</v>
@@ -781,7 +781,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -795,25 +795,25 @@
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
         <v>2</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O9">
         <v>33</v>
@@ -825,46 +825,46 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K10" t="s">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="N10">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O10">
         <v>33</v>

</xml_diff>

<commit_message>
animation normal boss + 1/2 camera
</commit_message>
<xml_diff>
--- a/Sprite Soures/temp_push.xlsx
+++ b/Sprite Soures/temp_push.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="13">
   <si>
     <t>=</t>
   </si>
@@ -31,6 +31,33 @@
   </si>
   <si>
     <t>temp.push_back(Rect(</t>
+  </si>
+  <si>
+    <t>Picture1</t>
+  </si>
+  <si>
+    <t>Picture2</t>
+  </si>
+  <si>
+    <t>Picture3</t>
+  </si>
+  <si>
+    <t>Picture4</t>
+  </si>
+  <si>
+    <t>Picture5</t>
+  </si>
+  <si>
+    <t>Picture6</t>
+  </si>
+  <si>
+    <t>Picture7</t>
+  </si>
+  <si>
+    <t>Picture8</t>
+  </si>
+  <si>
+    <t>Picture9</t>
   </si>
 </sst>
 </file>
@@ -351,7 +378,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,50 +392,50 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <f>M1</f>
-        <v>43</v>
+        <f t="shared" ref="B1:B19" si="0">M1</f>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1">
-        <f>L1</f>
-        <v>33</v>
+        <f t="shared" ref="D1:D19" si="1">L1</f>
+        <v>700</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1">
-        <f>M1+O1</f>
-        <v>45</v>
+        <f t="shared" ref="F1:F19" si="2">M1+O1</f>
+        <v>447</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1">
-        <f>L1+N1</f>
-        <v>35</v>
+        <f t="shared" ref="H1:H19" si="3">L1+N1</f>
+        <v>920</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1">
-        <v>0</v>
+      <c r="J1" t="s">
+        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
       </c>
       <c r="L1">
-        <v>33</v>
+        <v>700</v>
       </c>
       <c r="M1">
-        <v>43</v>
+        <v>227</v>
       </c>
       <c r="N1">
-        <v>2</v>
+        <v>220</v>
       </c>
       <c r="O1">
-        <v>2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -416,50 +443,50 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>M2</f>
-        <v>61</v>
+        <f t="shared" si="0"/>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <f>L2</f>
-        <v>65</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
-        <f>M2+O2</f>
-        <v>75</v>
+        <f t="shared" si="2"/>
+        <v>468</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2">
-        <f>L2+N2</f>
-        <v>79</v>
+        <f t="shared" si="3"/>
+        <v>233</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="J2" t="s">
+        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>61</v>
+        <v>235</v>
       </c>
       <c r="N2">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="O2">
-        <v>14</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -467,50 +494,50 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>M3</f>
-        <v>52</v>
+        <f t="shared" si="0"/>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
-        <f>L3</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>468</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
-        <f>M3+O3</f>
-        <v>76</v>
+        <f t="shared" si="2"/>
+        <v>457</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
-        <f>L3+N3</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>695</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>2</v>
+      <c r="J3" t="s">
+        <v>6</v>
       </c>
       <c r="K3" t="s">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>468</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>231</v>
       </c>
       <c r="N3">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="O3">
-        <v>24</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -518,50 +545,50 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>M4</f>
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
-        <f>L4</f>
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>234</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4">
-        <f>M4+O4</f>
-        <v>35</v>
+        <f t="shared" si="2"/>
+        <v>465</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
-        <f>L4+N4</f>
-        <v>67</v>
+        <f t="shared" si="3"/>
+        <v>465</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>3</v>
+      <c r="J4" t="s">
+        <v>7</v>
       </c>
       <c r="K4" t="s">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>39</v>
+        <v>234</v>
       </c>
       <c r="M4">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="N4">
-        <v>28</v>
+        <v>231</v>
       </c>
       <c r="O4">
-        <v>12</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -569,50 +596,50 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>M5</f>
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
-        <f>L5</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>468</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5">
-        <f>M5+O5</f>
-        <v>51</v>
+        <f t="shared" si="2"/>
+        <v>230</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
       <c r="H5">
-        <f>L5+N5</f>
-        <v>32</v>
+        <f t="shared" si="3"/>
+        <v>699</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="J5">
-        <v>4</v>
+      <c r="J5" t="s">
+        <v>8</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>468</v>
       </c>
       <c r="M5">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="O5">
-        <v>8</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -620,50 +647,50 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <f>M6</f>
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
-        <f>L6</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6">
-        <f>M6+O6</f>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>226</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
       </c>
       <c r="H6">
-        <f>L6+N6</f>
-        <v>38</v>
+        <f t="shared" si="3"/>
+        <v>926</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="J6">
-        <v>5</v>
+      <c r="J6" t="s">
+        <v>9</v>
       </c>
       <c r="K6" t="s">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="M6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="O6">
-        <v>12</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -671,50 +698,50 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <f>M7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7">
-        <f>L7</f>
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7">
-        <f>M7+O7</f>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>234</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
       <c r="H7">
-        <f>L7+N7</f>
-        <v>75</v>
+        <f t="shared" si="3"/>
+        <v>233</v>
       </c>
       <c r="I7" t="s">
         <v>2</v>
       </c>
-      <c r="J7">
-        <v>6</v>
+      <c r="J7" t="s">
+        <v>10</v>
       </c>
       <c r="K7" t="s">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>36</v>
+        <v>233</v>
       </c>
       <c r="O7">
-        <v>22</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -722,35 +749,35 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <f>M8</f>
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>469</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8">
-        <f>L8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8">
-        <f>M8+O8</f>
-        <v>42</v>
+        <f t="shared" si="2"/>
+        <v>689</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
       </c>
       <c r="H8">
-        <f>L8+N8</f>
-        <v>38</v>
+        <f t="shared" si="3"/>
+        <v>219</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
-      <c r="J8">
-        <v>7</v>
+      <c r="J8" t="s">
+        <v>11</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -759,13 +786,13 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>30</v>
+        <v>469</v>
       </c>
       <c r="N8">
-        <v>38</v>
+        <v>219</v>
       </c>
       <c r="O8">
-        <v>12</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -773,50 +800,50 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f>M9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <f>L9</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>234</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9">
-        <f>M9+O9</f>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>234</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
       </c>
       <c r="H9">
-        <f>L9+N9</f>
-        <v>38</v>
+        <f t="shared" si="3"/>
+        <v>467</v>
       </c>
       <c r="I9" t="s">
         <v>2</v>
       </c>
-      <c r="J9">
-        <v>8</v>
+      <c r="J9" t="s">
+        <v>12</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>234</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>38</v>
+        <v>233</v>
       </c>
       <c r="O9">
-        <v>16</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -824,28 +851,28 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <f>M10</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
-        <f>L10</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10">
-        <f>M10+O10</f>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
       </c>
       <c r="H10">
-        <f>L10+N10</f>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="I10" t="s">
@@ -875,28 +902,28 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <f>M11</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <f>L11</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11">
-        <f>M11+O11</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
       </c>
       <c r="H11">
-        <f>L11+N11</f>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="I11" t="s">
@@ -926,28 +953,28 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <f>M12</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12">
-        <f>L12</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12">
-        <f>M12+O12</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
       <c r="H12">
-        <f>L12+N12</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="I12" t="s">
@@ -977,28 +1004,28 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <f>M13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13">
-        <f>L13</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
       <c r="F13">
-        <f>M13+O13</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="G13" t="s">
         <v>1</v>
       </c>
       <c r="H13">
-        <f>L13+N13</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="I13" t="s">
@@ -1028,28 +1055,28 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <f>M14</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14">
-        <f>L14</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14">
-        <f>M14+O14</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="G14" t="s">
         <v>1</v>
       </c>
       <c r="H14">
-        <f>L14+N14</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="I14" t="s">
@@ -1079,28 +1106,28 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <f>M15</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15">
-        <f>L15</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15">
-        <f>M15+O15</f>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="G15" t="s">
         <v>1</v>
       </c>
       <c r="H15">
-        <f>L15+N15</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="I15" t="s">
@@ -1130,28 +1157,28 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <f>M16</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16">
-        <f>L16</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16">
-        <f>M16+O16</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>1</v>
       </c>
       <c r="H16">
-        <f>L16+N16</f>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="I16" t="s">
@@ -1181,28 +1208,28 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <f>M17</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17">
-        <f>L17</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
       <c r="F17">
-        <f>M17+O17</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
       <c r="H17">
-        <f>L17+N17</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="I17" t="s">
@@ -1232,28 +1259,28 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <f>M18</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18">
-        <f>L18</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
       </c>
       <c r="F18">
-        <f>M18+O18</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="G18" t="s">
         <v>1</v>
       </c>
       <c r="H18">
-        <f>L18+N18</f>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="I18" t="s">
@@ -1283,28 +1310,28 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <f>M19</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19">
-        <f>L19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
       <c r="F19">
-        <f>M19+O19</f>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="G19" t="s">
         <v>1</v>
       </c>
       <c r="H19">
-        <f>L19+N19</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="I19" t="s">

</xml_diff>

<commit_message>
1/2 camera on map
</commit_message>
<xml_diff>
--- a/Sprite Soures/temp_push.xlsx
+++ b/Sprite Soures/temp_push.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="8">
   <si>
     <t>=</t>
   </si>
@@ -31,21 +31,6 @@
   </si>
   <si>
     <t>temp.push_back(Rect(</t>
-  </si>
-  <si>
-    <t>Picture1</t>
-  </si>
-  <si>
-    <t>Picture2</t>
-  </si>
-  <si>
-    <t>Picture3</t>
-  </si>
-  <si>
-    <t>Picture4</t>
-  </si>
-  <si>
-    <t>Picture5</t>
   </si>
   <si>
     <t>Picture6</t>
@@ -378,7 +363,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:I9"/>
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,49 +378,49 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B19" si="0">M1</f>
-        <v>227</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1">
         <f t="shared" ref="D1:D19" si="1">L1</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1">
         <f t="shared" ref="F1:F19" si="2">M1+O1</f>
-        <v>447</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1">
         <f t="shared" ref="H1:H19" si="3">L1+N1</f>
-        <v>920</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
-        <v>4</v>
+      <c r="J1">
+        <v>0</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
       </c>
       <c r="L1">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="M1">
-        <v>227</v>
+        <v>0</v>
       </c>
       <c r="N1">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="O1">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -444,49 +429,49 @@
       </c>
       <c r="B2">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" si="2"/>
-        <v>468</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" si="3"/>
-        <v>233</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
-        <v>5</v>
+      <c r="J2">
+        <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M2">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>233</v>
+        <v>27</v>
       </c>
       <c r="O2">
-        <v>233</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -495,49 +480,49 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" si="2"/>
-        <v>457</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" si="3"/>
-        <v>695</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
-        <v>6</v>
+      <c r="J3">
+        <v>2</v>
       </c>
       <c r="K3" t="s">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>231</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>227</v>
+        <v>39</v>
       </c>
       <c r="O3">
-        <v>226</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -546,49 +531,49 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>465</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>465</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
-        <v>7</v>
+      <c r="J4">
+        <v>3</v>
       </c>
       <c r="K4" t="s">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>234</v>
+        <v>68</v>
       </c>
       <c r="M4">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>231</v>
+        <v>27</v>
       </c>
       <c r="O4">
-        <v>230</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -597,49 +582,49 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>699</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="J5" t="s">
-        <v>8</v>
+      <c r="J5">
+        <v>4</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="N5">
-        <v>231</v>
+        <v>24</v>
       </c>
       <c r="O5">
-        <v>230</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -675,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
         <v>0</v>
@@ -726,7 +711,7 @@
         <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K7" t="s">
         <v>0</v>
@@ -777,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -828,7 +813,7 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
health + destroy animation
</commit_message>
<xml_diff>
--- a/Sprite Soures/temp_push.xlsx
+++ b/Sprite Soures/temp_push.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="A1:I17"/>
+      <selection activeCell="I4" sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,29 +365,29 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <f>M1</f>
-        <v>64</v>
+        <f t="shared" ref="B1:B17" si="0">M1</f>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1">
-        <f>L1</f>
-        <v>201</v>
+        <f t="shared" ref="D1:D17" si="1">L1</f>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1">
-        <f>M1+O1</f>
-        <v>112</v>
+        <f t="shared" ref="F1:F17" si="2">M1+O1</f>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1">
-        <f>L1+N1</f>
-        <v>205</v>
+        <f t="shared" ref="H1:H17" si="3">L1+N1</f>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -399,16 +399,16 @@
         <v>0</v>
       </c>
       <c r="L1">
-        <v>201</v>
+        <v>17</v>
       </c>
       <c r="M1">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="N1">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O1">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -416,29 +416,29 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>M2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <f>L2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
-        <f>M2+O2</f>
-        <v>44</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2">
-        <f>L2+N2</f>
-        <v>46</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
@@ -456,10 +456,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="O2">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -467,29 +467,29 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>M3</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
-        <f>L3</f>
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
-        <f>M3+O3</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
-        <f>L3+N3</f>
-        <v>90</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
@@ -501,16 +501,16 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="N3">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="O3">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -518,29 +518,29 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>M4</f>
-        <v>82</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
-        <f>L4</f>
-        <v>88</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4">
-        <f>M4+O4</f>
-        <v>118</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
-        <f>L4+N4</f>
-        <v>126</v>
+        <f t="shared" si="3"/>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
@@ -552,16 +552,16 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="M4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="O4">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -569,28 +569,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>M5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
-        <f>L5</f>
+        <f t="shared" si="1"/>
         <v>174</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5">
-        <f>M5+O5</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
       <c r="H5">
-        <f>L5+N5</f>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="I5" t="s">
@@ -620,28 +620,28 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <f>M6</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
-        <f>L6</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6">
-        <f>M6+O6</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
       </c>
       <c r="H6">
-        <f>L6+N6</f>
+        <f t="shared" si="3"/>
         <v>167</v>
       </c>
       <c r="I6" t="s">
@@ -671,28 +671,28 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <f>M7</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7">
-        <f>L7</f>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7">
-        <f>M7+O7</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
       <c r="H7">
-        <f>L7+N7</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="I7" t="s">
@@ -722,28 +722,28 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <f>M8</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8">
-        <f>L8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8">
-        <f>M8+O8</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
       </c>
       <c r="H8">
-        <f>L8+N8</f>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="I8" t="s">
@@ -773,28 +773,28 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f>M9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <f>L9</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9">
-        <f>M9+O9</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
       </c>
       <c r="H9">
-        <f>L9+N9</f>
+        <f t="shared" si="3"/>
         <v>134</v>
       </c>
       <c r="I9" t="s">
@@ -824,28 +824,28 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <f>M10</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
-        <f>L10</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10">
-        <f>M10+O10</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
       </c>
       <c r="H10">
-        <f>L10+N10</f>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="I10" t="s">
@@ -875,28 +875,28 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <f>M11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <f>L11</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11">
-        <f>M11+O11</f>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
       </c>
       <c r="H11">
-        <f>L11+N11</f>
+        <f t="shared" si="3"/>
         <v>173</v>
       </c>
       <c r="I11" t="s">
@@ -926,28 +926,28 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <f>M12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12">
-        <f>L12</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12">
-        <f>M12+O12</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
       <c r="H12">
-        <f>L12+N12</f>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="I12" t="s">
@@ -977,28 +977,28 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <f>M13</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13">
-        <f>L13</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
       <c r="F13">
-        <f>M13+O13</f>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G13" t="s">
         <v>1</v>
       </c>
       <c r="H13">
-        <f>L13+N13</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="I13" t="s">
@@ -1028,28 +1028,28 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <f>M14</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14">
-        <f>L14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14">
-        <f>M14+O14</f>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="G14" t="s">
         <v>1</v>
       </c>
       <c r="H14">
-        <f>L14+N14</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="I14" t="s">
@@ -1079,28 +1079,28 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <f>M15</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15">
-        <f>L15</f>
+        <f t="shared" si="1"/>
         <v>174</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15">
-        <f>M15+O15</f>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="G15" t="s">
         <v>1</v>
       </c>
       <c r="H15">
-        <f>L15+N15</f>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="I15" t="s">
@@ -1130,28 +1130,28 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <f>M16</f>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16">
-        <f>L16</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16">
-        <f>M16+O16</f>
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="G16" t="s">
         <v>1</v>
       </c>
       <c r="H16">
-        <f>L16+N16</f>
+        <f t="shared" si="3"/>
         <v>159</v>
       </c>
       <c r="I16" t="s">
@@ -1181,28 +1181,28 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <f>M17</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17">
-        <f>L17</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
       <c r="F17">
-        <f>M17+O17</f>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
       <c r="H17">
-        <f>L17+N17</f>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="I17" t="s">

</xml_diff>